<commit_message>
openpyxl - manipulando as planilhas do Workbook
</commit_message>
<xml_diff>
--- a/Modulos_Python/aula199/workbook.xlsx
+++ b/Modulos_Python/aula199/workbook.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Minha planilha" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -458,7 +458,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C3" t="n">
         <v>9.699999999999999</v>

</xml_diff>